<commit_message>
Finish data description file
</commit_message>
<xml_diff>
--- a/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
+++ b/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoeniger\Documents\Github\EEG-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF3715-5A29-47BE-83C8-887EE5557DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7E2AF5-B231-4CC1-8353-C23B4275F665}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" activeTab="1" xr2:uid="{2A34AAA6-619F-46F9-9F22-5EEF8FB60B91}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Reservoir capacity (MWh storage capacity/MW installed capacity)</t>
   </si>
@@ -72,51 +72,6 @@
   </si>
   <si>
     <t>Initial transmission capacity between regions</t>
-  </si>
-  <si>
-    <t>Investment cost in new transmission capacity</t>
-  </si>
-  <si>
-    <t>Transmission cost between region</t>
-  </si>
-  <si>
-    <t>Transmission loss between regions (fraction)</t>
-  </si>
-  <si>
-    <t>Variation of the water inflow to reservoirs</t>
-  </si>
-  <si>
-    <t>Weekly variation of generation of hydro run-of-river</t>
-  </si>
-  <si>
-    <t>Annual net electricity export to third regions</t>
-  </si>
-  <si>
-    <t>Taxes €/MWh Fuel Used For Electricity Production</t>
-  </si>
-  <si>
-    <t>Taxes €/MWh Fuel Used For Heat Production</t>
-  </si>
-  <si>
-    <t>Taxes €/MWh Fuel Used For Electricity Production in CHP</t>
-  </si>
-  <si>
-    <t>Taxes €/MWh Fuel Used For Heat Production in CHP</t>
-  </si>
-  <si>
-    <t>Heat demand profile</t>
-  </si>
-  <si>
-    <t>Electricity demand profile</t>
-  </si>
-  <si>
-    <t>Wind generation profile</t>
-  </si>
-  <si>
-    <t>Solar power generation profile</t>
-  </si>
-  <si>
-    <t>Solar heat generation profile</t>
   </si>
   <si>
     <t>Name</t>
@@ -246,13 +201,73 @@
   </si>
   <si>
     <t>Annual brutto heat consumption</t>
+  </si>
+  <si>
+    <t>CHP heat demand (PRIMES)</t>
+  </si>
+  <si>
+    <t>Heat demand based on PRIMES euco30 with own adaptations to meet 2030 targets (on RES and EE)</t>
+  </si>
+  <si>
+    <t>TABLE XKFX(YYY,IRRRE,IRRRI)</t>
+  </si>
+  <si>
+    <t>TYNDP2018</t>
+  </si>
+  <si>
+    <t>Distributed generation scenario for 2040; linearly interpolated between 2020 and 2040</t>
+  </si>
+  <si>
+    <t>Transmission loss</t>
+  </si>
+  <si>
+    <t>TABLE XLOSS(IRRRE,IRRRI)</t>
+  </si>
+  <si>
+    <t>Fuel prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE FUELPRICE1(YYY,RRR,FFF) </t>
+  </si>
+  <si>
+    <t>only values in black are included by us, red was there before</t>
+  </si>
+  <si>
+    <t>IEA WEO 2016 for fossil fuel price trends and</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SET-Nav Diversification pathway for carbon price (using fuel prices as input)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE M_POL(YYY,MPOLSET,CCC)  </t>
+  </si>
+  <si>
+    <t>CO2 price</t>
+  </si>
+  <si>
+    <t>Renewable profiles</t>
+  </si>
+  <si>
+    <t>demand profiles</t>
+  </si>
+  <si>
+    <t>Hireps</t>
+  </si>
+  <si>
+    <t>weather year 2008</t>
+  </si>
+  <si>
+    <t>51,52</t>
+  </si>
+  <si>
+    <t>all data in red is dummy data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,19 +310,20 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -326,7 +342,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -338,6 +353,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -395,8 +411,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25F218B9-07B1-4295-84A3-40E9ACBEB053}" name="Tabelle1" displayName="Tabelle1" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10" xr:uid="{6687B5F8-02B0-43C8-B509-81FC2C86B0B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25F218B9-07B1-4295-84A3-40E9ACBEB053}" name="Tabelle1" displayName="Tabelle1" ref="A1:F19" totalsRowShown="0">
+  <autoFilter ref="A1:F19" xr:uid="{6687B5F8-02B0-43C8-B509-81FC2C86B0B7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{608B8B6C-5F09-4625-A118-36507CDD1A8A}" name="Tab"/>
     <tableColumn id="2" xr3:uid="{66CE98BA-7D3B-469A-B3A1-37C293F30BD6}" name="What"/>
@@ -405,7 +421,7 @@
     <tableColumn id="4" xr3:uid="{42F3E22E-915C-46FB-9A64-65D5A364E252}" name="Source"/>
     <tableColumn id="5" xr3:uid="{CC806C10-F04F-4809-82C7-A0A3864DAA22}" name="Remarks"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -715,35 +731,35 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>19</v>
+      <c r="A1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>48</v>
+      <c r="A3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -755,38 +771,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A715C67D-2C69-43F3-B600-37CB9534AA1C}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="28.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="76.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -794,30 +810,30 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -826,12 +842,12 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="6">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5">
         <v>0.05</v>
       </c>
       <c r="F4" s="1"/>
@@ -841,12 +857,12 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4">
         <v>8.0199999999999994E-2</v>
       </c>
       <c r="F5" s="1"/>
@@ -856,12 +872,12 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="5">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
@@ -871,12 +887,12 @@
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="5">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F7" s="1"/>
@@ -886,177 +902,236 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="5">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4">
         <v>0.1</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="7"/>
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="6"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>58</v>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="6"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
</commit_message>
<xml_diff>
--- a/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
+++ b/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoeniger\Documents\Github\EEG-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1641FB-8879-409A-9AA4-A32275280F35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306AC167-5EBF-4199-8FAC-B92FA26CFB56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" xr2:uid="{2A34AAA6-619F-46F9-9F22-5EEF8FB60B91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" activeTab="1" xr2:uid="{2A34AAA6-619F-46F9-9F22-5EEF8FB60B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -60,15 +60,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>Reservoir capacity (MWh storage capacity/MW installed capacity)</t>
   </si>
   <si>
     <t>Minimum and maximum values of hydro storage levels</t>
-  </si>
-  <si>
-    <t>Weekly CHP production profile</t>
   </si>
   <si>
     <t>Initial transmission capacity between regions</t>
@@ -724,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A63FC0-51B6-4226-9FC8-A25EE4BD4855}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -732,34 +729,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -771,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A715C67D-2C69-43F3-B600-37CB9534AA1C}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,22 +784,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -810,14 +807,14 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -826,14 +823,14 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -842,10 +839,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="5">
         <v>0.05</v>
@@ -857,10 +854,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="4">
         <v>8.0199999999999994E-2</v>
@@ -872,10 +869,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -887,10 +884,10 @@
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4">
         <v>3.2000000000000001E-2</v>
@@ -902,10 +899,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4">
         <v>0.1</v>
@@ -917,42 +914,42 @@
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="6"/>
       <c r="F11" s="1"/>
@@ -962,35 +959,33 @@
         <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -998,17 +993,17 @@
         <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,10 +1011,10 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D15" s="6">
         <v>2.1999999999999999E-2</v>
@@ -1031,17 +1026,17 @@
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,49 +1044,49 @@
         <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="6"/>
       <c r="E18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="6"/>
       <c r="E19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>

</xml_diff>

<commit_message>
Update data description and units in data input file
</commit_message>
<xml_diff>
--- a/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
+++ b/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoeniger\Documents\Github\EEG-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A230D22B-009D-41FE-851F-08F14590A19A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993250FF-2C43-472B-B574-D1E39969E4F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" activeTab="1" xr2:uid="{2A34AAA6-619F-46F9-9F22-5EEF8FB60B91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10428" activeTab="1" xr2:uid="{2A34AAA6-619F-46F9-9F22-5EEF8FB60B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -223,12 +223,6 @@
     <t>only values in black are included by us, red was there before</t>
   </si>
   <si>
-    <t>IEA WEO 2016 for fossil fuel price trends and</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SET-Nav Diversification pathway for carbon price (using fuel prices as input)</t>
-  </si>
-  <si>
     <t xml:space="preserve">TABLE M_POL(YYY,MPOLSET,CCC)  </t>
   </si>
   <si>
@@ -258,6 +252,12 @@
   <si>
     <t>Conventional plants: diploma thesis of Marcel Hanke
 Sources: costs (PRIMES https://ec.europa.eu/energy/sites/ener/files/documents/2018_06_27_technology_pathways_-_finalreportmain2.pdf), cv and cb values (Danish Energy Agency https://ens.dk/sites/ens.dk/files/Statistik/technology_data_catalogue_for_el_and_dh_-_0008.pdf)</t>
+  </si>
+  <si>
+    <t>SET-Nav Diversification pathway for carbon price (using fuel prices as input) [EUR2015] (originally from AURES II offshore case study)</t>
+  </si>
+  <si>
+    <t>IEA WEO 2016 for fossil fuel price trends [EUR2015] (originally from the AURES II offshore case study)</t>
   </si>
 </sst>
 </file>
@@ -725,9 +725,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -735,7 +735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -743,15 +743,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -769,20 +769,20 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="76.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="85.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="76.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -802,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -818,7 +818,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -830,11 +830,11 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -849,7 +849,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -864,7 +864,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>21</v>
       </c>
@@ -879,7 +879,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -894,7 +894,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>25</v>
       </c>
@@ -909,7 +909,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>28</v>
       </c>
@@ -923,7 +923,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -941,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -954,7 +954,7 @@
       <c r="D11" s="6"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>33</v>
       </c>
@@ -970,7 +970,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>34</v>
       </c>
@@ -988,7 +988,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>35</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>38</v>
       </c>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>39</v>
       </c>
@@ -1033,99 +1033,99 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="6"/>
       <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="6"/>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F32" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include costs info in description files
</commit_message>
<xml_diff>
--- a/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
+++ b/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoeniger\Documents\Github\EEG-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368ABD7F-5622-443B-A20A-DCE512A6A118}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20DC67E-ABFA-4734-9946-027A76B8BCBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>Reservoir capacity (MWh storage capacity/MW installed capacity)</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>2020: TYNDP2018 Distributed Generation Scenario; 2030 + 2040: TYNDP2020 National Trends Scenario (2040: Reference Grid plus Extended Grid)</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>EUR_2015</t>
   </si>
 </sst>
 </file>
@@ -1072,15 +1078,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1104,12 +1110,20 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1121,21 +1135,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="76.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="85.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="76.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1155,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -1171,7 +1185,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -1187,7 +1201,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -1202,7 +1216,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1217,7 +1231,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>21</v>
       </c>
@@ -1232,7 +1246,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -1247,7 +1261,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>25</v>
       </c>
@@ -1262,7 +1276,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>28</v>
       </c>
@@ -1276,7 +1290,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1294,7 +1308,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1307,7 +1321,7 @@
       <c r="D11" s="6"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>33</v>
       </c>
@@ -1323,7 +1337,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>34</v>
       </c>
@@ -1341,7 +1355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>35</v>
       </c>
@@ -1357,7 +1371,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>38</v>
       </c>
@@ -1372,7 +1386,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>39</v>
       </c>
@@ -1390,7 +1404,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>40</v>
       </c>
@@ -1406,7 +1420,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
@@ -1419,7 +1433,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -1435,7 +1449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>58</v>
       </c>
@@ -1443,40 +1457,40 @@
       <c r="D20" s="6"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F32" s="1"/>
     </row>
   </sheetData>
@@ -1496,9 +1510,9 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>63</v>
       </c>
@@ -1514,7 +1528,7 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>64</v>
       </c>
@@ -1557,7 +1571,7 @@
         <v>7.3342749999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>66</v>
       </c>
@@ -1600,7 +1614,7 @@
         <v>48.406214999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>67</v>
       </c>
@@ -1643,7 +1657,7 @@
         <v>28.885760000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>68</v>
       </c>
@@ -1679,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="62.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
@@ -1722,7 +1736,7 @@
         <v>33.737665</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
@@ -1739,7 +1753,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2020</v>
       </c>
@@ -1756,7 +1770,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
@@ -1773,7 +1787,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2040</v>
       </c>
@@ -1790,7 +1804,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2050</v>
       </c>
@@ -1807,7 +1821,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1822,7 +1836,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2020</v>
       </c>
@@ -1840,7 +1854,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2030</v>
       </c>
@@ -1858,7 +1872,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2040</v>
       </c>
@@ -1876,7 +1890,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2050</v>
       </c>
@@ -1894,43 +1908,43 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="15"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update costs to EUR_2020
- Update costs from EUR_2015 to EUR_2020 in tab 16,17,39,40, and 50_1.
- Fix bugs (missing boiler technologies in tab 5 and 6).
</commit_message>
<xml_diff>
--- a/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
+++ b/Data_description_Input_Austria_2030 (compatible with current BB4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoeniger\Documents\Github\EEG-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20DC67E-ABFA-4734-9946-027A76B8BCBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E948321A-0CB2-4A64-9091-7E651D30A1C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -252,12 +252,6 @@
 Sources: costs (PRIMES https://ec.europa.eu/energy/sites/ener/files/documents/2018_06_27_technology_pathways_-_finalreportmain2.pdf), cv and cb values (Danish Energy Agency https://ens.dk/sites/ens.dk/files/Statistik/technology_data_catalogue_for_el_and_dh_-_0008.pdf)</t>
   </si>
   <si>
-    <t>SET-Nav Diversification pathway for carbon price (using fuel prices as input) [EUR2015] (originally from AURES II offshore case study)</t>
-  </si>
-  <si>
-    <t>IEA WEO 2016 for fossil fuel price trends [EUR2015] (originally from the AURES II offshore case study)</t>
-  </si>
-  <si>
     <t>Preisannahmen</t>
   </si>
   <si>
@@ -326,7 +320,13 @@
     <t>Costs</t>
   </si>
   <si>
-    <t>EUR_2015</t>
+    <t>EUR_2020</t>
+  </si>
+  <si>
+    <t>IEA WEO 2016 for fossil fuel price trends [EUR2020] (originally from the AURES II offshore case study)</t>
+  </si>
+  <si>
+    <t>SET-Nav Diversification pathway for carbon price (using fuel prices as input) [EUR2020] (originally from AURES II offshore case study)</t>
   </si>
 </sst>
 </file>
@@ -1080,13 +1080,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1118,12 +1118,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1135,21 +1135,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="76.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="85.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="76.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>21</v>
       </c>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>25</v>
       </c>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>28</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1321,7 +1321,7 @@
       <c r="D11" s="6"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>33</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>34</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>35</v>
       </c>
@@ -1367,11 +1367,11 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>38</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>39</v>
       </c>
@@ -1398,13 +1398,13 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>40</v>
       </c>
@@ -1416,11 +1416,11 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>58</v>
       </c>
@@ -1457,40 +1457,40 @@
       <c r="D20" s="6"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
     </row>
   </sheetData>
@@ -1510,11 +1510,11 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="10"/>
@@ -1528,12 +1528,12 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$12</f>
@@ -1571,12 +1571,12 @@
         <v>7.3342749999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$13</f>
@@ -1614,12 +1614,12 @@
         <v>48.406214999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$14</f>
@@ -1657,12 +1657,12 @@
         <v>28.885760000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="13">
         <v>4</v>
@@ -1693,12 +1693,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="62.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$15</f>
@@ -1736,24 +1736,24 @@
         <v>33.737665</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2020</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2040</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2050</v>
       </c>
@@ -1821,22 +1821,22 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2020</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2030</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2040</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2050</v>
       </c>
@@ -1908,43 +1908,43 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="15"/>
     </row>
   </sheetData>

</xml_diff>